<commit_message>
Add email and sms codes.
</commit_message>
<xml_diff>
--- a/doc/task.xlsx
+++ b/doc/task.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>说明</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -310,10 +310,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Service组件完成  总进度50%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>数据库初始化数据  总进度100%</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -345,8 +341,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +486,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -497,9 +496,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -517,7 +513,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -591,7 +587,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -626,7 +621,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -802,21 +796,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="14.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.5" customWidth="1"/>
     <col min="4" max="4" width="45.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
@@ -824,8 +818,8 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -836,8 +830,8 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="81" x14ac:dyDescent="0.15">
-      <c r="A3" s="14"/>
+    <row r="3" spans="1:4" ht="81">
+      <c r="A3" s="11"/>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -846,8 +840,8 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="14"/>
+    <row r="4" spans="1:4" ht="67.5">
+      <c r="A4" s="11"/>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -855,11 +849,11 @@
         <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="14"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="40.5">
+      <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -868,8 +862,8 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:4" ht="27">
+      <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -880,8 +874,8 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A7" s="14"/>
+    <row r="7" spans="1:4" ht="67.5">
+      <c r="A7" s="11"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -890,8 +884,8 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -904,8 +898,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:4">
+      <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -914,8 +908,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="14"/>
+    <row r="10" spans="1:4">
+      <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
@@ -924,8 +918,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:4">
+      <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
@@ -934,8 +928,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="14"/>
+    <row r="12" spans="1:4">
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -943,11 +937,11 @@
         <v>23</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="14"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="11"/>
       <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
@@ -955,11 +949,11 @@
         <v>25</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="14"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="11"/>
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
@@ -968,8 +962,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -979,11 +973,11 @@
         <v>29</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="14"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="11"/>
       <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
@@ -991,11 +985,11 @@
         <v>31</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="14"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="11"/>
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1003,11 +997,11 @@
         <v>33</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="14"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1015,11 +1009,11 @@
         <v>35</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="14"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="11"/>
       <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1027,11 +1021,11 @@
         <v>37</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="14"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
@@ -1039,11 +1033,11 @@
         <v>39</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="12" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1052,35 +1046,35 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
+    <row r="22" spans="1:4">
+      <c r="A22" s="13"/>
       <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="12"/>
+    <row r="23" spans="1:4">
+      <c r="A23" s="13"/>
       <c r="B23" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A24" s="13"/>
+    <row r="24" spans="1:4" ht="27">
+      <c r="A24" s="14"/>
       <c r="B24" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="40.5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:4" ht="40.5" hidden="1">
+      <c r="A25" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1088,49 +1082,49 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" ht="40.5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="12"/>
+    <row r="26" spans="1:4" ht="40.5" hidden="1">
+      <c r="A26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:4" ht="94.5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="14"/>
-      <c r="B27" s="12"/>
+    <row r="27" spans="1:4" ht="94.5" hidden="1">
+      <c r="A27" s="11"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="14"/>
-      <c r="B28" s="12"/>
+    <row r="28" spans="1:4" hidden="1">
+      <c r="A28" s="11"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="14"/>
-      <c r="B29" s="12"/>
+    <row r="29" spans="1:4" hidden="1">
+      <c r="A29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" ht="54" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="14"/>
-      <c r="B30" s="13"/>
+    <row r="30" spans="1:4" ht="54" hidden="1">
+      <c r="A30" s="11"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" ht="54" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="14"/>
-      <c r="B31" s="11" t="s">
+    <row r="31" spans="1:4" ht="54" hidden="1">
+      <c r="A31" s="11"/>
+      <c r="B31" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -1138,27 +1132,27 @@
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="14"/>
-      <c r="B32" s="12"/>
+    <row r="32" spans="1:4" hidden="1">
+      <c r="A32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4" ht="67.5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="14"/>
-      <c r="B33" s="13"/>
+    <row r="33" spans="1:4" ht="67.5" hidden="1">
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="11" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -1166,45 +1160,45 @@
       </c>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="12"/>
-      <c r="B35" s="14"/>
+    <row r="35" spans="1:4">
+      <c r="A35" s="13"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="12"/>
-      <c r="B36" s="14"/>
+    <row r="36" spans="1:4">
+      <c r="A36" s="13"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="12"/>
-      <c r="B37" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="13"/>
+      <c r="B37" s="11" t="s">
         <v>61</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="12"/>
-      <c r="B38" s="14"/>
+    <row r="38" spans="1:4">
+      <c r="A38" s="13"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="13"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="14"/>
       <c r="B39" s="3" t="s">
         <v>64</v>
       </c>
@@ -1212,22 +1206,22 @@
         <v>65</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A24"/>
     <mergeCell ref="B25:B30"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="A34:A39"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="A25:A33"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1236,12 +1230,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1249,12 +1243,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add query category customers.
</commit_message>
<xml_diff>
--- a/doc/task.xlsx
+++ b/doc/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>说明</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -335,6 +335,14 @@
 奖品发放
 --&gt;query 100%,service有问题
 --&gt;insert 100%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Service完成  总进度50%
+2.无法实现
+3.Service完成  总进度50%
+4.Service完成  总进度50%
+发短信,发邮件  =&gt;  Service完成  总进度50%</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -486,9 +494,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -496,6 +501,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -799,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -819,7 +827,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -831,17 +839,19 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="81">
-      <c r="A3" s="11"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="67.5">
-      <c r="A4" s="11"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -853,7 +863,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="40.5">
-      <c r="A5" s="11"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -863,7 +873,7 @@
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="27">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -875,7 +885,7 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="67.5">
-      <c r="A7" s="11"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -885,7 +895,7 @@
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -899,7 +909,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="11"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -909,7 +919,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="11"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
@@ -919,7 +929,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="11"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
@@ -929,7 +939,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="11"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -941,7 +951,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="11"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
@@ -953,7 +963,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="11"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
@@ -963,7 +973,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -977,7 +987,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="11"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
@@ -989,7 +999,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="11"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1001,7 +1011,7 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="11"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1013,7 +1023,7 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="11"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1025,7 +1035,7 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="11"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
@@ -1037,7 +1047,7 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1047,7 +1057,7 @@
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="13"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
@@ -1055,7 +1065,7 @@
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="13"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="3" t="s">
         <v>43</v>
       </c>
@@ -1063,7 +1073,7 @@
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" ht="27">
-      <c r="A24" s="14"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="5" t="s">
         <v>44</v>
       </c>
@@ -1071,10 +1081,10 @@
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" ht="40.5" hidden="1">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1083,48 +1093,48 @@
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" ht="40.5" hidden="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="13"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" ht="94.5" hidden="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" hidden="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" hidden="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="54" hidden="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" ht="54" hidden="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12" t="s">
+      <c r="A31" s="14"/>
+      <c r="B31" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -1133,26 +1143,26 @@
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" hidden="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" ht="67.5" hidden="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="14"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D33" s="8"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -1161,16 +1171,16 @@
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="13"/>
-      <c r="B35" s="11"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="13"/>
-      <c r="B36" s="11"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="4" t="s">
         <v>60</v>
       </c>
@@ -1179,8 +1189,8 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="13"/>
-      <c r="B37" s="11" t="s">
+      <c r="A37" s="12"/>
+      <c r="B37" s="14" t="s">
         <v>61</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -1188,8 +1198,8 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="13"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="4" t="s">
         <v>63</v>
       </c>
@@ -1198,7 +1208,7 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="14"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="3" t="s">
         <v>64</v>
       </c>
@@ -1211,17 +1221,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A24"/>
     <mergeCell ref="B25:B30"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="A34:A39"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="A25:A33"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>